<commit_message>
update load main lenh san xuat + tien do giao hang
</commit_message>
<xml_diff>
--- a/src/main/webapp/TemplateUpload/Template_ChaoGia_New.xlsx
+++ b/src/main/webapp/TemplateUpload/Template_ChaoGia_New.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\GMESApiCore\src\main\webapp\TemplateUpload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\GMES_API\GMESApiCore\src\main\webapp\TemplateUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FC8068-23FA-4B8E-8DAB-E0A84964FBD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7997887-037A-4338-98DE-677D3D48D5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,12 @@
     <sheet name="Mô tả" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TemplateN1AA61" hidden="1">Template!$N$1:$W$2</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TemplateN1AA61" hidden="1">Template!$O$1:$X$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +55,7 @@
     <author>Nguyễn Hồng Phong</author>
   </authors>
   <commentList>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{1FCED54E-AA08-4F68-8226-F582A79B36AD}">
+    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{1FCED54E-AA08-4F68-8226-F582A79B36AD}">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Infant</t>
   </si>
@@ -228,39 +228,6 @@
     <t>Style (Set) (3)</t>
   </si>
   <si>
-    <t>Mã SP (Buyer) (4)</t>
-  </si>
-  <si>
-    <t>Tên Sản phẩm (5)</t>
-  </si>
-  <si>
-    <t>Số lượng SP trong bộ (6)</t>
-  </si>
-  <si>
-    <t>Ngày NPL về (7)</t>
-  </si>
-  <si>
-    <t>Phương thức vận chuyển (8)</t>
-  </si>
-  <si>
-    <t>ĐV chính (9)</t>
-  </si>
-  <si>
-    <t>Trạng thái (10)</t>
-  </si>
-  <si>
-    <t>Vendor Target (11)</t>
-  </si>
-  <si>
-    <t>Giá FOB (12)</t>
-  </si>
-  <si>
-    <t>NS Target (13)</t>
-  </si>
-  <si>
-    <t>xxx (14)</t>
-  </si>
-  <si>
     <t>\</t>
   </si>
   <si>
@@ -295,18 +262,53 @@
   </si>
   <si>
     <t>Đợt 2</t>
+  </si>
+  <si>
+    <t>Style (set vendor) (4)</t>
+  </si>
+  <si>
+    <t>Mã SP (Buyer) (5)</t>
+  </si>
+  <si>
+    <t>Tên Sản phẩm (6)</t>
+  </si>
+  <si>
+    <t>Số lượng SP trong bộ (7)</t>
+  </si>
+  <si>
+    <t>Ngày NPL về (8)</t>
+  </si>
+  <si>
+    <t>Phương thức vận chuyển (9)</t>
+  </si>
+  <si>
+    <t>ĐV chính (10)</t>
+  </si>
+  <si>
+    <t>Trạng thái (11)</t>
+  </si>
+  <si>
+    <t>Vendor Target (12)</t>
+  </si>
+  <si>
+    <t>Giá FOB (13)</t>
+  </si>
+  <si>
+    <t>NS Target (14)</t>
+  </si>
+  <si>
+    <t>xxx (15)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,8 +339,14 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +380,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -483,39 +497,47 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,7 +559,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nguyễn Hồng Phong" refreshedDate="44188.980249768516" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5" xr:uid="{870425F1-E360-4853-B79B-5ED6B1B051BC}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="N1:W2" sheet="Template"/>
+    <worksheetSource ref="O1:X2" sheet="Template"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="xxx (14)" numFmtId="0">
@@ -777,7 +799,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F5C0102B-07BE-4D85-80ED-98A93B6485F0}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F5C0102B-07BE-4D85-80ED-98A93B6485F0}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E4" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="5">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -860,7 +882,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0AC633C-5F0E-469A-ADAF-9CC6E0480E29}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0AC633C-5F0E-469A-ADAF-9CC6E0480E29}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="H5:L6" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="12">
     <pivotField showAll="0">
@@ -1255,319 +1277,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM24"/>
+  <dimension ref="A1:AV24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U2" sqref="U1:U1048576"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="16" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="16" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" style="16" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" customWidth="1"/>
-    <col min="23" max="23" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.28515625" customWidth="1"/>
-    <col min="29" max="29" width="8.5703125" customWidth="1"/>
-    <col min="30" max="30" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="4" style="10" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="14" width="9.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="16" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" style="16" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" style="16" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" customWidth="1"/>
+    <col min="24" max="24" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.28515625" customWidth="1"/>
+    <col min="30" max="30" width="8.5703125" customWidth="1"/>
+    <col min="31" max="31" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:48" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="24"/>
+      <c r="T1" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="24"/>
+      <c r="V1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="24"/>
+      <c r="X1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" s="27"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="Q3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="X3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3"/>
+      <c r="AF3" s="16"/>
+      <c r="AH3" s="10"/>
+      <c r="AL3"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="19"/>
+      <c r="AV3" s="10"/>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="Q4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="X4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4"/>
+      <c r="AF4" s="16"/>
+      <c r="AH4" s="10"/>
+      <c r="AL4"/>
+      <c r="AO4" s="10"/>
+      <c r="AP4" s="19"/>
+      <c r="AV4" s="10"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="Q5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="X5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5"/>
+      <c r="AF5" s="16"/>
+      <c r="AH5" s="10"/>
+      <c r="AL5"/>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="19"/>
+      <c r="AV5" s="10"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="Q6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="X6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6"/>
+      <c r="AF6" s="16"/>
+      <c r="AH6" s="10"/>
+      <c r="AL6"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="19"/>
+      <c r="AV6" s="10"/>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="Q7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="X7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7"/>
+      <c r="AF7" s="16"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="20"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7"/>
+      <c r="AO7" s="10"/>
+      <c r="AP7" s="19"/>
+      <c r="AV7" s="10"/>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="Q8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="X8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8"/>
+      <c r="AF8" s="16"/>
+      <c r="AH8" s="10"/>
+      <c r="AL8"/>
+      <c r="AO8" s="10"/>
+      <c r="AP8" s="19"/>
+      <c r="AV8" s="10"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="Q9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="X9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9"/>
+      <c r="AF9" s="16"/>
+      <c r="AH9" s="10"/>
+      <c r="AL9"/>
+      <c r="AO9" s="10"/>
+      <c r="AP9" s="19"/>
+      <c r="AV9" s="10"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="Q10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="X10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AB10" s="16"/>
+      <c r="AD10" s="16"/>
+      <c r="AE10"/>
+      <c r="AF10" s="16"/>
+      <c r="AH10" s="10"/>
+      <c r="AL10"/>
+      <c r="AO10" s="10"/>
+      <c r="AP10" s="19"/>
+      <c r="AV10" s="10"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AM11" s="11"/>
+      <c r="AN11" s="14"/>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AM12" s="11"/>
+      <c r="AN12" s="14"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AM13" s="11"/>
+      <c r="AN13" s="14"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="14"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="14"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="14"/>
+    </row>
+    <row r="17" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AM17" s="11"/>
+      <c r="AN17" s="14"/>
+    </row>
+    <row r="18" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AB18" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="V1" s="26"/>
-      <c r="W1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE1" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="W2" s="13"/>
-      <c r="X2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK2" s="17"/>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL3" s="11"/>
-      <c r="AM3" s="14"/>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="14"/>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL5" s="11"/>
-      <c r="AM5" s="14"/>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL6" s="11"/>
-      <c r="AM6" s="14"/>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL7" s="11"/>
-      <c r="AM7" s="14"/>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="14"/>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="14"/>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL10" s="11"/>
-      <c r="AM10" s="14"/>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL11" s="11"/>
-      <c r="AM11" s="14"/>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="14"/>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="14"/>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL14" s="11"/>
-      <c r="AM14" s="14"/>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="14"/>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="AL16" s="11"/>
-      <c r="AM16" s="14"/>
-    </row>
-    <row r="17" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AL17" s="11"/>
-      <c r="AM17" s="14"/>
-    </row>
-    <row r="18" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AA18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL18" s="11"/>
-      <c r="AM18" s="14"/>
-    </row>
-    <row r="19" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AL19" s="11"/>
-      <c r="AM19" s="14"/>
-    </row>
-    <row r="20" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AL20" s="11"/>
-      <c r="AM20" s="14"/>
-    </row>
-    <row r="21" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AL21" s="11"/>
-      <c r="AM21" s="14"/>
-    </row>
-    <row r="22" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="14"/>
-    </row>
-    <row r="23" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AL23" s="11"/>
-      <c r="AM23" s="14"/>
-    </row>
-    <row r="24" spans="27:39" x14ac:dyDescent="0.25">
-      <c r="AL24" s="11"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="14"/>
+    </row>
+    <row r="19" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AM19" s="11"/>
+      <c r="AN19" s="14"/>
+    </row>
+    <row r="20" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AM20" s="11"/>
+      <c r="AN20" s="14"/>
+    </row>
+    <row r="21" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AM21" s="11"/>
+      <c r="AN21" s="14"/>
+    </row>
+    <row r="22" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AM22" s="11"/>
+      <c r="AN22" s="14"/>
+    </row>
+    <row r="23" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AM23" s="11"/>
+      <c r="AN23" s="14"/>
+    </row>
+    <row r="24" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AM24" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="M1:M2"/>
+  <mergeCells count="22">
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="AE1:AJ1"/>
-    <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="X1:AC1"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1580,7 +1738,7 @@
           <x14:formula1>
             <xm:f>'Mô tả'!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J8:J1048576 J3:J6</xm:sqref>
+          <xm:sqref>K11:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1604,19 +1762,19 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,19 +1851,19 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="L5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>